<commit_message>
updated full to publish final file
</commit_message>
<xml_diff>
--- a/wk29temp.xlsx
+++ b/wk29temp.xlsx
@@ -624,7 +624,7 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
@@ -1094,7 +1094,7 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M11" t="n">
         <v>0</v>
@@ -1316,7 +1316,7 @@
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
       <c r="L15" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M15" t="n">
         <v>1</v>
@@ -1951,7 +1951,7 @@
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
       <c r="L26" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M26" t="n">
         <v>0</v>
@@ -2002,7 +2002,7 @@
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
       <c r="L27" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M27" t="n">
         <v>0</v>
@@ -3198,7 +3198,7 @@
       <c r="J47" t="inlineStr"/>
       <c r="K47" t="inlineStr"/>
       <c r="L47" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M47" t="n">
         <v>0</v>
@@ -3353,7 +3353,7 @@
       <c r="J50" t="inlineStr"/>
       <c r="K50" t="inlineStr"/>
       <c r="L50" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M50" t="n">
         <v>0</v>
@@ -4035,7 +4035,7 @@
       <c r="J62" t="inlineStr"/>
       <c r="K62" t="inlineStr"/>
       <c r="L62" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M62" t="n">
         <v>0</v>
@@ -4743,7 +4743,7 @@
       <c r="J74" t="inlineStr"/>
       <c r="K74" t="inlineStr"/>
       <c r="L74" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M74" t="n">
         <v>0</v>
@@ -5441,7 +5441,7 @@
       <c r="J86" t="inlineStr"/>
       <c r="K86" t="inlineStr"/>
       <c r="L86" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M86" t="n">
         <v>0</v>
@@ -5858,7 +5858,7 @@
       <c r="J93" t="inlineStr"/>
       <c r="K93" t="inlineStr"/>
       <c r="L93" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M93" t="n">
         <v>1</v>
@@ -6137,7 +6137,7 @@
       <c r="J98" t="inlineStr"/>
       <c r="K98" t="inlineStr"/>
       <c r="L98" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M98" t="n">
         <v>0</v>
@@ -6849,7 +6849,7 @@
       <c r="J110" t="inlineStr"/>
       <c r="K110" t="inlineStr"/>
       <c r="L110" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M110" t="n">
         <v>0</v>
@@ -6900,7 +6900,7 @@
       <c r="J111" t="inlineStr"/>
       <c r="K111" t="inlineStr"/>
       <c r="L111" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M111" t="n">
         <v>1</v>
@@ -7539,7 +7539,7 @@
       <c r="J122" t="inlineStr"/>
       <c r="K122" t="inlineStr"/>
       <c r="L122" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M122" t="n">
         <v>0</v>
@@ -7590,7 +7590,7 @@
       <c r="J123" t="inlineStr"/>
       <c r="K123" t="inlineStr"/>
       <c r="L123" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M123" t="n">
         <v>1</v>
@@ -7952,7 +7952,7 @@
       <c r="J129" t="inlineStr"/>
       <c r="K129" t="inlineStr"/>
       <c r="L129" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M129" t="n">
         <v>1</v>
@@ -8005,7 +8005,7 @@
       <c r="J130" t="inlineStr"/>
       <c r="K130" t="inlineStr"/>
       <c r="L130" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M130" t="n">
         <v>0</v>
@@ -8231,7 +8231,7 @@
       <c r="J134" t="inlineStr"/>
       <c r="K134" t="inlineStr"/>
       <c r="L134" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M134" t="n">
         <v>0</v>
@@ -8284,7 +8284,7 @@
       <c r="J135" t="inlineStr"/>
       <c r="K135" t="inlineStr"/>
       <c r="L135" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M135" t="n">
         <v>1</v>
@@ -8705,7 +8705,7 @@
       <c r="J142" t="inlineStr"/>
       <c r="K142" t="inlineStr"/>
       <c r="L142" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M142" t="n">
         <v>0</v>
@@ -8758,7 +8758,7 @@
       <c r="J143" t="inlineStr"/>
       <c r="K143" t="inlineStr"/>
       <c r="L143" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M143" t="n">
         <v>0</v>
@@ -8917,7 +8917,7 @@
       <c r="J146" t="inlineStr"/>
       <c r="K146" t="inlineStr"/>
       <c r="L146" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M146" t="n">
         <v>0</v>
@@ -9344,7 +9344,7 @@
       <c r="J153" t="inlineStr"/>
       <c r="K153" t="inlineStr"/>
       <c r="L153" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M153" t="n">
         <v>1</v>
@@ -9397,7 +9397,7 @@
       <c r="J154" t="inlineStr"/>
       <c r="K154" t="inlineStr"/>
       <c r="L154" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M154" t="n">
         <v>0</v>
@@ -9623,7 +9623,7 @@
       <c r="J158" t="inlineStr"/>
       <c r="K158" t="inlineStr"/>
       <c r="L158" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M158" t="n">
         <v>0</v>
@@ -10093,7 +10093,7 @@
       <c r="J166" t="inlineStr"/>
       <c r="K166" t="inlineStr"/>
       <c r="L166" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M166" t="n">
         <v>0</v>
@@ -10319,7 +10319,7 @@
       <c r="J170" t="inlineStr"/>
       <c r="K170" t="inlineStr"/>
       <c r="L170" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M170" t="n">
         <v>0</v>
@@ -10805,7 +10805,7 @@
       <c r="J178" t="inlineStr"/>
       <c r="K178" t="inlineStr"/>
       <c r="L178" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M178" t="n">
         <v>0</v>
@@ -10858,7 +10858,7 @@
       <c r="J179" t="inlineStr"/>
       <c r="K179" t="inlineStr"/>
       <c r="L179" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M179" t="n">
         <v>0</v>
@@ -11015,7 +11015,7 @@
       <c r="J182" t="inlineStr"/>
       <c r="K182" t="inlineStr"/>
       <c r="L182" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M182" t="n">
         <v>0</v>
@@ -11703,7 +11703,7 @@
       <c r="J194" t="inlineStr"/>
       <c r="K194" t="inlineStr"/>
       <c r="L194" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M194" t="n">
         <v>0</v>
@@ -11754,7 +11754,7 @@
       <c r="J195" t="inlineStr"/>
       <c r="K195" t="inlineStr"/>
       <c r="L195" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M195" t="n">
         <v>0</v>
@@ -12220,7 +12220,7 @@
       <c r="J203" t="inlineStr"/>
       <c r="K203" t="inlineStr"/>
       <c r="L203" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M203" t="n">
         <v>0</v>
@@ -12375,7 +12375,7 @@
       <c r="J206" t="inlineStr"/>
       <c r="K206" t="inlineStr"/>
       <c r="L206" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M206" t="n">
         <v>0</v>
@@ -13075,7 +13075,7 @@
       <c r="J218" t="inlineStr"/>
       <c r="K218" t="inlineStr"/>
       <c r="L218" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M218" t="n">
         <v>0</v>
@@ -13547,7 +13547,7 @@
       <c r="J226" t="inlineStr"/>
       <c r="K226" t="inlineStr"/>
       <c r="L226" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M226" t="n">
         <v>0</v>
@@ -13753,7 +13753,7 @@
       <c r="J230" t="inlineStr"/>
       <c r="K230" t="inlineStr"/>
       <c r="L230" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M230" t="n">
         <v>0</v>
@@ -14225,7 +14225,7 @@
       <c r="J238" t="inlineStr"/>
       <c r="K238" t="inlineStr"/>
       <c r="L238" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M238" t="n">
         <v>0</v>
@@ -14278,7 +14278,7 @@
       <c r="J239" t="inlineStr"/>
       <c r="K239" t="inlineStr"/>
       <c r="L239" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M239" t="n">
         <v>0</v>
@@ -14433,7 +14433,7 @@
       <c r="J242" t="inlineStr"/>
       <c r="K242" t="inlineStr"/>
       <c r="L242" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M242" t="n">
         <v>0</v>
@@ -14852,7 +14852,7 @@
       <c r="J249" t="inlineStr"/>
       <c r="K249" t="inlineStr"/>
       <c r="L249" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M249" t="n">
         <v>1</v>
@@ -14968,7 +14968,7 @@
       <c r="J251" t="inlineStr"/>
       <c r="K251" t="inlineStr"/>
       <c r="L251" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M251" t="n">
         <v>0</v>
@@ -15121,7 +15121,7 @@
       <c r="J254" t="inlineStr"/>
       <c r="K254" t="inlineStr"/>
       <c r="L254" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M254" t="n">
         <v>0</v>
@@ -16256,7 +16256,7 @@
       <c r="J273" t="inlineStr"/>
       <c r="K273" t="inlineStr"/>
       <c r="L273" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M273" t="n">
         <v>1</v>
@@ -16586,7 +16586,7 @@
       <c r="J279" t="inlineStr"/>
       <c r="K279" t="inlineStr"/>
       <c r="L279" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M279" t="n">
         <v>0</v>
@@ -17274,7 +17274,7 @@
       <c r="J291" t="inlineStr"/>
       <c r="K291" t="inlineStr"/>
       <c r="L291" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M291" t="n">
         <v>1</v>
@@ -17634,7 +17634,7 @@
       <c r="J297" t="inlineStr"/>
       <c r="K297" t="inlineStr"/>
       <c r="L297" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M297" t="n">
         <v>1</v>
@@ -19036,7 +19036,7 @@
       <c r="J321" t="inlineStr"/>
       <c r="K321" t="inlineStr"/>
       <c r="L321" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M321" t="n">
         <v>1</v>
@@ -19740,7 +19740,7 @@
       <c r="J333" t="inlineStr"/>
       <c r="K333" t="inlineStr"/>
       <c r="L333" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M333" t="n">
         <v>1</v>
@@ -20440,7 +20440,7 @@
       <c r="J345" t="inlineStr"/>
       <c r="K345" t="inlineStr"/>
       <c r="L345" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M345" t="n">
         <v>1</v>
@@ -20493,7 +20493,7 @@
       <c r="J346" t="inlineStr"/>
       <c r="K346" t="inlineStr"/>
       <c r="L346" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M346" t="n">
         <v>0</v>
@@ -21140,7 +21140,7 @@
       <c r="J357" t="inlineStr"/>
       <c r="K357" t="inlineStr"/>
       <c r="L357" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M357" t="n">
         <v>1</v>
@@ -21193,7 +21193,7 @@
       <c r="J358" t="inlineStr"/>
       <c r="K358" t="inlineStr"/>
       <c r="L358" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M358" t="n">
         <v>0</v>
@@ -21838,7 +21838,7 @@
       <c r="J369" t="inlineStr"/>
       <c r="K369" t="inlineStr"/>
       <c r="L369" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M369" t="n">
         <v>1</v>
@@ -21891,7 +21891,7 @@
       <c r="J370" t="inlineStr"/>
       <c r="K370" t="inlineStr"/>
       <c r="L370" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M370" t="n">
         <v>0</v>
@@ -22591,7 +22591,7 @@
       <c r="J382" t="inlineStr"/>
       <c r="K382" t="inlineStr"/>
       <c r="L382" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M382" t="n">
         <v>0</v>
@@ -22866,7 +22866,7 @@
       <c r="J387" t="inlineStr"/>
       <c r="K387" t="inlineStr"/>
       <c r="L387" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M387" t="n">
         <v>0</v>
@@ -23228,7 +23228,7 @@
       <c r="J393" t="inlineStr"/>
       <c r="K393" t="inlineStr"/>
       <c r="L393" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M393" t="n">
         <v>1</v>
@@ -23910,7 +23910,7 @@
       <c r="J405" t="inlineStr"/>
       <c r="K405" t="inlineStr"/>
       <c r="L405" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M405" t="n">
         <v>1</v>
@@ -24610,7 +24610,7 @@
       <c r="J417" t="inlineStr"/>
       <c r="K417" t="inlineStr"/>
       <c r="L417" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M417" t="n">
         <v>1</v>
@@ -25664,7 +25664,7 @@
       <c r="J435" t="inlineStr"/>
       <c r="K435" t="inlineStr"/>
       <c r="L435" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M435" t="n">
         <v>1</v>
@@ -26350,7 +26350,7 @@
       <c r="J447" t="inlineStr"/>
       <c r="K447" t="inlineStr"/>
       <c r="L447" s="2" t="n">
-        <v>45147.77649364964</v>
+        <v>45148.53813368532</v>
       </c>
       <c r="M447" t="n">
         <v>1</v>

</xml_diff>